<commit_message>
sửa tên đt xiaomi
</commit_message>
<xml_diff>
--- a/DATABASE/CSDL.xlsx
+++ b/DATABASE/CSDL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATT\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9664D743-C681-4E05-A020-A4BA111B1BB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F3D83E-7FD4-4E77-9AFE-C6E8FB40866F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12720" firstSheet="5" activeTab="7" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12720" firstSheet="6" activeTab="13" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
   </bookViews>
   <sheets>
     <sheet name="MODEL" sheetId="1" r:id="rId1"/>
@@ -229,24 +229,9 @@
     <t>poco x3 nfc</t>
   </si>
   <si>
-    <t>note 9s</t>
-  </si>
-  <si>
-    <t>note 9t</t>
-  </si>
-  <si>
-    <t>note 9</t>
-  </si>
-  <si>
     <t>redmi note 9</t>
   </si>
   <si>
-    <t>redmi note 9t</t>
-  </si>
-  <si>
-    <t>redmi note 9c</t>
-  </si>
-  <si>
     <t>find x2</t>
   </si>
   <si>
@@ -320,6 +305,21 @@
   </si>
   <si>
     <t>internet banking</t>
+  </si>
+  <si>
+    <t>redmi note 9PRO</t>
+  </si>
+  <si>
+    <t>redmi 9</t>
+  </si>
+  <si>
+    <t>redmi 9t</t>
+  </si>
+  <si>
+    <t>redmi 9c</t>
+  </si>
+  <si>
+    <t>redmi note 9s</t>
   </si>
 </sst>
 </file>
@@ -854,15 +854,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA133F23-BFFC-4B9C-BEB3-BF235ED8168F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.9140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -879,7 +879,7 @@
         <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -893,10 +893,10 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -910,10 +910,10 @@
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -927,10 +927,10 @@
         <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -944,10 +944,10 @@
         <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -961,10 +961,10 @@
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -975,13 +975,13 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -992,13 +992,13 @@
         <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1009,13 +1009,13 @@
         <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1026,13 +1026,13 @@
         <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1043,13 +1043,13 @@
         <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1220,7 +1220,7 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -1235,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC5A483-2E88-42E7-AE63-B1A73126D6ED}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1257,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1265,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done 25 sản phẩm
</commit_message>
<xml_diff>
--- a/DATABASE/CSDL.xlsx
+++ b/DATABASE/CSDL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATT\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F3D83E-7FD4-4E77-9AFE-C6E8FB40866F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570CBBB0-861E-4415-BDCA-6B1634435ADE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12720" firstSheet="6" activeTab="13" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
   </bookViews>
@@ -855,7 +855,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
use case user + đặc tả yêu cầu
</commit_message>
<xml_diff>
--- a/DATABASE/CSDL.xlsx
+++ b/DATABASE/CSDL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoangLam\Desktop\DATABASE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ĐỒ ÁN TỐT NGHIỆP\DATT\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4637276-BC46-45A2-8CB2-EAACE3954F97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FE51C3-84C6-4FE0-B9D3-551DE79574BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="11" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAI" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
   <si>
     <t>apple</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>CauHinh</t>
   </si>
 </sst>
 </file>
@@ -669,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E907879-2CF0-4084-BEBA-930BAEAE93DE}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA133F23-BFFC-4B9C-BEB3-BF235ED8168F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -981,7 +984,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,7 +1018,7 @@
         <v>70</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="J1" t="s">
         <v>71</v>
@@ -1069,7 +1072,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
cập nhật lược đồ, CSDL
</commit_message>
<xml_diff>
--- a/DATABASE/CSDL.xlsx
+++ b/DATABASE/CSDL.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ĐỒ ÁN TỐT NGHIỆP\DATT\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341D104C-E7BF-42A1-ABA5-541F1A8447F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1F5E84-5658-4D60-9CAA-BF67F320479C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="3" activeTab="4" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="7" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
   </bookViews>
   <sheets>
-    <sheet name="LOAISP" sheetId="1" r:id="rId1"/>
-    <sheet name="DIENTHOAI" sheetId="2" r:id="rId2"/>
-    <sheet name="NHACUNGCAP" sheetId="3" r:id="rId3"/>
-    <sheet name="KHUYENMAI" sheetId="4" r:id="rId4"/>
-    <sheet name="CTKM" sheetId="15" r:id="rId5"/>
-    <sheet name="HOADON" sheetId="5" r:id="rId6"/>
-    <sheet name="PTTT" sheetId="14" r:id="rId7"/>
+    <sheet name="NHACUNGCAP" sheetId="3" r:id="rId1"/>
+    <sheet name="BAOHANH" sheetId="17" r:id="rId2"/>
+    <sheet name="MAUSP" sheetId="1" r:id="rId3"/>
+    <sheet name="SANPHAM" sheetId="2" r:id="rId4"/>
+    <sheet name="DANHGIA" sheetId="16" r:id="rId5"/>
+    <sheet name="KHUYENMAI" sheetId="4" r:id="rId6"/>
+    <sheet name="DONHANG" sheetId="5" r:id="rId7"/>
     <sheet name="CTHD" sheetId="6" r:id="rId8"/>
-    <sheet name="TAIKHOAN" sheetId="7" r:id="rId9"/>
-    <sheet name="BINHLUAN" sheetId="8" r:id="rId10"/>
-    <sheet name="KHO" sheetId="9" r:id="rId11"/>
+    <sheet name="PTTT" sheetId="14" r:id="rId9"/>
+    <sheet name="TAIKHOAN" sheetId="7" r:id="rId10"/>
+    <sheet name="BINHLUAN" sheetId="8" r:id="rId11"/>
     <sheet name="SLIDESHOW" sheetId="10" r:id="rId12"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId13"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t>apple</t>
   </si>
@@ -213,12 +213,6 @@
     <t>mi 10t pro 5g</t>
   </si>
   <si>
-    <t>MaLoai</t>
-  </si>
-  <si>
-    <t>TenLoai</t>
-  </si>
-  <si>
     <t>MoTa</t>
   </si>
   <si>
@@ -258,21 +252,12 @@
     <t>DiaChi</t>
   </si>
   <si>
-    <t>SDt</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>MaHD</t>
-  </si>
-  <si>
     <t>ThoiGian</t>
   </si>
   <si>
-    <t>MaKH</t>
-  </si>
-  <si>
     <t>MaPTTT</t>
   </si>
   <si>
@@ -291,12 +276,6 @@
     <t>HoTen</t>
   </si>
   <si>
-    <t>Matkhau</t>
-  </si>
-  <si>
-    <t>TaiKhoan</t>
-  </si>
-  <si>
     <t>AnhDaiDien</t>
   </si>
   <si>
@@ -306,9 +285,6 @@
     <t>NoiDung</t>
   </si>
   <si>
-    <t>SLNhap</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
@@ -339,16 +315,37 @@
     <t>MaBL</t>
   </si>
   <si>
-    <t>MaKho</t>
-  </si>
-  <si>
     <t>TenPTTT</t>
   </si>
   <si>
-    <t>MaCT</t>
-  </si>
-  <si>
     <t>MaSP</t>
+  </si>
+  <si>
+    <t>MaMau</t>
+  </si>
+  <si>
+    <t>TenMau</t>
+  </si>
+  <si>
+    <t>TenSP</t>
+  </si>
+  <si>
+    <t>MaDH</t>
+  </si>
+  <si>
+    <t>MatKhau</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>NgayMua</t>
+  </si>
+  <si>
+    <t>TGBH</t>
+  </si>
+  <si>
+    <t>IMEI</t>
   </si>
 </sst>
 </file>
@@ -700,117 +697,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E907879-2CF0-4084-BEBA-930BAEAE93DE}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5864F5-B45D-4530-A131-7E628563F6BD}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508042DB-84D0-4BC9-A327-C88757AD0B18}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35483A1-0DF5-43CF-90E4-2ADCD3378A81}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7AE07C-EA68-47D0-B94C-895BE7C6388D}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -823,20 +818,20 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1052,49 +1047,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2508716E-7333-40BE-B725-486EF949E833}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB46C4C-9EB7-482D-9E96-525FA1BD4CF9}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1103,36 +1085,103 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5864F5-B45D-4530-A131-7E628563F6BD}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E907879-2CF0-4084-BEBA-930BAEAE93DE}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
         <v>61</v>
       </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2508716E-7333-40BE-B725-486EF949E833}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1189,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BC2F3E-5B57-48E4-B6E4-C9FB9438508D}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29912F7-7002-454A-BB7B-FFAF709E890B}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1158,22 +1236,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1181,38 +1259,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F68FDC-99BB-4E71-A5BE-4EB88D10CE43}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5C4FB6-396C-45F8-AFFA-36AA2B8FB199}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,25 +1276,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1302,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2084C816-F8BC-4AD1-BA3F-7DFDF8DD9304}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC5A483-2E88-42E7-AE63-B1A73126D6ED}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1265,10 +1352,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1293,91 +1380,6 @@
       </c>
       <c r="B4" t="s">
         <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2084C816-F8BC-4AD1-BA3F-7DFDF8DD9304}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508042DB-84D0-4BC9-A327-C88757AD0B18}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thêm hình ảnh slideshow, thay đổi cấu trúc thư mục hình ảnh
</commit_message>
<xml_diff>
--- a/DATABASE/CSDL.xlsx
+++ b/DATABASE/CSDL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ĐỒ ÁN TỐT NGHIỆP\DATT\DATABASE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ĐỒ ÁN\DATT\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1F5E84-5658-4D60-9CAA-BF67F320479C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76966AE3-DBA1-4DC1-9CEE-B9EC6476C697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="7" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="12" xr2:uid="{A1F4E252-54F7-4355-89F1-293F14DA519F}"/>
   </bookViews>
   <sheets>
     <sheet name="NHACUNGCAP" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
   <si>
     <t>apple</t>
   </si>
@@ -105,9 +105,6 @@
     <t>mi 11 5g</t>
   </si>
   <si>
-    <t>note 9 pro</t>
-  </si>
-  <si>
     <t>poco x3 nfc</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>internet banking</t>
   </si>
   <si>
-    <t>redmi note 9PRO</t>
-  </si>
-  <si>
     <t>redmi 9</t>
   </si>
   <si>
@@ -346,6 +340,9 @@
   </si>
   <si>
     <t>IMEI</t>
+  </si>
+  <si>
+    <t>redmi note 9 pro</t>
   </si>
 </sst>
 </file>
@@ -356,7 +353,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -704,29 +701,29 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -742,35 +739,35 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" t="s">
-        <v>80</v>
-      </c>
       <c r="H1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -786,26 +783,26 @@
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>91</v>
       </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -821,17 +818,17 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -843,18 +840,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA133F23-BFFC-4B9C-BEB3-BF235ED8168F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -868,10 +865,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -882,13 +879,13 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -896,16 +893,16 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -916,13 +913,13 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -933,13 +930,13 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -947,16 +944,16 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -964,50 +961,50 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>55</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1015,30 +1012,27 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1054,29 +1048,29 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1092,35 +1086,35 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1137,51 +1131,51 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" t="s">
         <v>67</v>
-      </c>
-      <c r="J1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1197,20 +1191,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1226,32 +1220,32 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" t="s">
-        <v>89</v>
-      </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1267,34 +1261,34 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" t="s">
-        <v>74</v>
-      </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1306,30 +1300,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2084C816-F8BC-4AD1-BA3F-7DFDF8DD9304}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1345,41 +1339,41 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>